<commit_message>
New types of test
</commit_message>
<xml_diff>
--- a/cypress/downloads/ConciliacaoVendaSistema.xlsx
+++ b/cypress/downloads/ConciliacaoVendaSistema.xlsx
@@ -95,511 +95,511 @@
     <t>-</t>
   </si>
   <si>
+    <t>32D1FF57C3465172B62CC82F402F0622</t>
+  </si>
+  <si>
+    <t>00 / 00</t>
+  </si>
+  <si>
+    <t>Não localizado</t>
+  </si>
+  <si>
+    <t>Venda Sistema não localizada na operadora</t>
+  </si>
+  <si>
+    <t>E-COMMERCE</t>
+  </si>
+  <si>
+    <t>11268176</t>
+  </si>
+  <si>
+    <t>65181-BFD43-DD8-D65</t>
+  </si>
+  <si>
+    <t>Bin</t>
+  </si>
+  <si>
+    <t>AGIPLAN CREDITO A VISTA</t>
+  </si>
+  <si>
+    <t>ELO CREDITO - GETNET</t>
+  </si>
+  <si>
+    <t>0001 12345</t>
+  </si>
+  <si>
+    <t>01 / 01</t>
+  </si>
+  <si>
+    <t>ACSGerente</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>9606</t>
+  </si>
+  <si>
+    <t>VISA CREDITO A VISTA</t>
+  </si>
+  <si>
+    <t>VISA DEBITO - GETNET</t>
+  </si>
+  <si>
+    <t>000001123</t>
+  </si>
+  <si>
+    <t>9605</t>
+  </si>
+  <si>
+    <t>1A65480F4347E4E8C38CEFEEE52CA9F3</t>
+  </si>
+  <si>
+    <t>11080622</t>
+  </si>
+  <si>
+    <t>64FB1-A7C8A-D74-DB8</t>
+  </si>
+  <si>
+    <t>C01622135F5EF40E10646684687B8270</t>
+  </si>
+  <si>
+    <t>11082337</t>
+  </si>
+  <si>
+    <t>64FC5-41165-5D6-3BB</t>
+  </si>
+  <si>
+    <t>FED867E875EE7E62BADD93C4B17B4BBE</t>
+  </si>
+  <si>
+    <t>11096134</t>
+  </si>
+  <si>
+    <t>64FDB-F159E-79E-038</t>
+  </si>
+  <si>
+    <t>Pacote de 30.00 créditos</t>
+  </si>
+  <si>
+    <t>E4011FFE1B19AE5675F9D9FFF9A82CB3</t>
+  </si>
+  <si>
+    <t>11242936</t>
+  </si>
+  <si>
+    <t>65147-EDB3D-EBB-FA1</t>
+  </si>
+  <si>
+    <t>7BD2C04EC6750CF97ABAFD08743345E7</t>
+  </si>
+  <si>
+    <t>11248727</t>
+  </si>
+  <si>
+    <t>65156-51066-6A4-634</t>
+  </si>
+  <si>
+    <t>DB0C5D02EC4F40182EF0C1678436CD1D</t>
+  </si>
+  <si>
+    <t>11255547</t>
+  </si>
+  <si>
+    <t>6516B-D62C1-03E-3BA</t>
+  </si>
+  <si>
+    <t>351FE9D535C7DF757E4F5C0B30C92D11</t>
+  </si>
+  <si>
+    <t>11115004</t>
+  </si>
+  <si>
+    <t>65019-A327B-FEE-6EF</t>
+  </si>
+  <si>
+    <t>AF27F66082883F5765B5B36A3C21EA1D</t>
+  </si>
+  <si>
+    <t>11126261</t>
+  </si>
+  <si>
+    <t>65030-83F1B-D53-D15</t>
+  </si>
+  <si>
+    <t>6E01C8E62307266E17735C8B6F36C7DA</t>
+  </si>
+  <si>
+    <t>11138947</t>
+  </si>
+  <si>
+    <t>65045-4DEC1-12D-0A3</t>
+  </si>
+  <si>
+    <t>C20519E1E9FDEAB8181D243CE09685C1</t>
+  </si>
+  <si>
+    <t>11147494</t>
+  </si>
+  <si>
+    <t>65059-B42BA-D19-FD1</t>
+  </si>
+  <si>
+    <t>BC65C502E5110C98366953A867BD5EA</t>
+  </si>
+  <si>
+    <t>11154373</t>
+  </si>
+  <si>
+    <t>6506E-6FEE7-A0D-AA9</t>
+  </si>
+  <si>
+    <t>51B7EA171FDCF7F2B064FBFBC57AF911</t>
+  </si>
+  <si>
+    <t>11162057</t>
+  </si>
+  <si>
+    <t>65083-5B30F-D08-3F1</t>
+  </si>
+  <si>
+    <t>Pacote de 100.00 créditos</t>
+  </si>
+  <si>
+    <t>2947085C7B7D47C8A6C52C593B7A1B</t>
+  </si>
+  <si>
+    <t>11165975</t>
+  </si>
+  <si>
+    <t>6508A-EE673-40D-D9F</t>
+  </si>
+  <si>
+    <t>7B5F9F537E4A95B3CD73C46CCEEBE5D6</t>
+  </si>
+  <si>
+    <t>11170321</t>
+  </si>
+  <si>
+    <t>65098-957DA-3C7-FE6</t>
+  </si>
+  <si>
+    <t>735E439D4ADEBD265FCC7C71E8E54F25</t>
+  </si>
+  <si>
+    <t>11185239</t>
+  </si>
+  <si>
+    <t>650AF-98F68-B49-7F0</t>
+  </si>
+  <si>
+    <t>ED0EE50944F264F593925EB221C5D9E7</t>
+  </si>
+  <si>
+    <t>11192642</t>
+  </si>
+  <si>
+    <t>650C4-464BC-F67-D2F</t>
+  </si>
+  <si>
+    <t>FE3753775779E0EBE4F528393773DF2F</t>
+  </si>
+  <si>
+    <t>11199885</t>
+  </si>
+  <si>
+    <t>650D8-B0D5C-340-CF1</t>
+  </si>
+  <si>
+    <t>MAESTRO</t>
+  </si>
+  <si>
+    <t>3216354</t>
+  </si>
+  <si>
+    <t>2132132132</t>
+  </si>
+  <si>
+    <t>2754394</t>
+  </si>
+  <si>
+    <t>ELO CREDITO</t>
+  </si>
+  <si>
+    <t>32165416</t>
+  </si>
+  <si>
+    <t>32154651</t>
+  </si>
+  <si>
+    <t>2754397</t>
+  </si>
+  <si>
+    <t>32165132</t>
+  </si>
+  <si>
+    <t>3213431</t>
+  </si>
+  <si>
+    <t>2754400</t>
+  </si>
+  <si>
+    <t>1314351</t>
+  </si>
+  <si>
+    <t>3215431</t>
+  </si>
+  <si>
+    <t>2754402</t>
+  </si>
+  <si>
+    <t>500052</t>
+  </si>
+  <si>
+    <t>1015620</t>
+  </si>
+  <si>
+    <t>01 / 08</t>
+  </si>
+  <si>
+    <t>PDV</t>
+  </si>
+  <si>
+    <t>20002304242023002</t>
+  </si>
+  <si>
+    <t>500055</t>
+  </si>
+  <si>
+    <t>1015622</t>
+  </si>
+  <si>
+    <t>20002304342023002</t>
+  </si>
+  <si>
+    <t>500059</t>
+  </si>
+  <si>
+    <t>2010906</t>
+  </si>
+  <si>
+    <t>01 / 03</t>
+  </si>
+  <si>
+    <t>20002304582023002</t>
+  </si>
+  <si>
+    <t>20002304242023004</t>
+  </si>
+  <si>
+    <t>02 / 08</t>
+  </si>
+  <si>
+    <t>20002304242023005</t>
+  </si>
+  <si>
+    <t>03 / 08</t>
+  </si>
+  <si>
+    <t>20002304242023006</t>
+  </si>
+  <si>
+    <t>04 / 08</t>
+  </si>
+  <si>
+    <t>20002304242023007</t>
+  </si>
+  <si>
+    <t>05 / 08</t>
+  </si>
+  <si>
+    <t>20002304242023008</t>
+  </si>
+  <si>
+    <t>06 / 08</t>
+  </si>
+  <si>
+    <t>20002304242023009</t>
+  </si>
+  <si>
+    <t>07 / 08</t>
+  </si>
+  <si>
+    <t>20002304242023010</t>
+  </si>
+  <si>
+    <t>20002304582023004</t>
+  </si>
+  <si>
+    <t>02 / 03</t>
+  </si>
+  <si>
+    <t>20002304582023005</t>
+  </si>
+  <si>
+    <t>500098</t>
+  </si>
+  <si>
+    <t>2010932</t>
+  </si>
+  <si>
+    <t>01 / 04</t>
+  </si>
+  <si>
+    <t>20002306782023003</t>
+  </si>
+  <si>
+    <t>02 / 04</t>
+  </si>
+  <si>
+    <t>20002306782023004</t>
+  </si>
+  <si>
+    <t>03 / 04</t>
+  </si>
+  <si>
+    <t>20002306782023005</t>
+  </si>
+  <si>
+    <t>04 / 04</t>
+  </si>
+  <si>
+    <t>20002306782023006</t>
+  </si>
+  <si>
+    <t>MASTER CREDITO</t>
+  </si>
+  <si>
+    <t>AMEX - STONE</t>
+  </si>
+  <si>
+    <t>0000000001</t>
+  </si>
+  <si>
+    <t>9634</t>
+  </si>
+  <si>
+    <t>0000000123</t>
+  </si>
+  <si>
+    <t>9632</t>
+  </si>
+  <si>
+    <t>VISA ELECTRON DEBITO A VISTA</t>
+  </si>
+  <si>
+    <t>MASTERCARD CRED - GETNET</t>
+  </si>
+  <si>
+    <t>0000189852</t>
+  </si>
+  <si>
+    <t>9683</t>
+  </si>
+  <si>
+    <t>0000432268</t>
+  </si>
+  <si>
+    <t>9684</t>
+  </si>
+  <si>
+    <t>MASTERCARD DEB - GETNET</t>
+  </si>
+  <si>
+    <t>0000fr6rY6</t>
+  </si>
+  <si>
+    <t>9685</t>
+  </si>
+  <si>
+    <t>ELO DEBITO - GETNET</t>
+  </si>
+  <si>
+    <t>0000001234</t>
+  </si>
+  <si>
+    <t>9633</t>
+  </si>
+  <si>
+    <t>0000000002</t>
+  </si>
+  <si>
+    <t>9635</t>
+  </si>
+  <si>
+    <t>VISA CREDITO - GETNET</t>
+  </si>
+  <si>
+    <t>0000864432</t>
+  </si>
+  <si>
+    <t>9686</t>
+  </si>
+  <si>
+    <t>86D53E69155262C8FCFD2EF63FE27853</t>
+  </si>
+  <si>
+    <t>11220347</t>
+  </si>
+  <si>
+    <t>65117-34715-511-D1B</t>
+  </si>
+  <si>
+    <t>8C117FEA9E2E4B6EA2A5BB2262966F03</t>
+  </si>
+  <si>
+    <t>11230786</t>
+  </si>
+  <si>
+    <t>6512C-F1AB6-4FF-89A</t>
+  </si>
+  <si>
+    <t>71126DC5F86386E887EA54EB75D55444</t>
+  </si>
+  <si>
+    <t>11237663</t>
+  </si>
+  <si>
+    <t>65140-BA551-908-7FE</t>
+  </si>
+  <si>
+    <t>6B048F9AE4BAA59788A02EFFF74310D3</t>
+  </si>
+  <si>
+    <t>Divergente</t>
+  </si>
+  <si>
+    <t>Operadora - Operadora: VR - Sistema: Cielo&lt;br/&gt;Taxa - Operadora: 6,81 - Sistema: 2,32&lt;br/&gt;Valor Líquido - Operadora: 9,31 - Sistema: 0,00</t>
+  </si>
+  <si>
+    <t>11104464</t>
+  </si>
+  <si>
+    <t>64FF1-AB3A3-E4D-BF6</t>
+  </si>
+  <si>
+    <t>9BC101484C547842101FED2C34BA9204</t>
+  </si>
+  <si>
+    <t>Operadora - Operadora: Ticket - Sistema: Cielo&lt;br/&gt;Taxa - Operadora: 6,02 - Sistema: 2,32&lt;br/&gt;Valor Líquido - Operadora: 9,53 - Sistema: 0,00</t>
+  </si>
+  <si>
+    <t>11108858</t>
+  </si>
+  <si>
+    <t>65005-C7684-990-C99</t>
+  </si>
+  <si>
     <t>C3B1F34D39C6A551D38E119B15CD9884</t>
   </si>
   <si>
-    <t>00 / 00</t>
-  </si>
-  <si>
-    <t>Divergente</t>
-  </si>
-  <si>
     <t>Operadora - Operadora: Ticket - Sistema: Cielo&lt;br/&gt;Taxa - Operadora: 5,97 - Sistema: 2,32&lt;br/&gt;Valor Líquido - Operadora: 8,67 - Sistema: 0,00</t>
   </si>
   <si>
-    <t>E-COMMERCE</t>
-  </si>
-  <si>
     <t>11068299</t>
   </si>
   <si>
     <t>64F86-F75C5-C9C-E7E</t>
-  </si>
-  <si>
-    <t>Bin</t>
-  </si>
-  <si>
-    <t>AGIPLAN CREDITO A VISTA</t>
-  </si>
-  <si>
-    <t>ELO CREDITO - GETNET</t>
-  </si>
-  <si>
-    <t>0001 12345</t>
-  </si>
-  <si>
-    <t>01 / 01</t>
-  </si>
-  <si>
-    <t>Não localizado</t>
-  </si>
-  <si>
-    <t>Venda Sistema não localizada na operadora</t>
-  </si>
-  <si>
-    <t>ACSGerente</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>9606</t>
-  </si>
-  <si>
-    <t>VISA CREDITO A VISTA</t>
-  </si>
-  <si>
-    <t>VISA DEBITO - GETNET</t>
-  </si>
-  <si>
-    <t>000001123</t>
-  </si>
-  <si>
-    <t>9605</t>
-  </si>
-  <si>
-    <t>1A65480F4347E4E8C38CEFEEE52CA9F3</t>
-  </si>
-  <si>
-    <t>11080622</t>
-  </si>
-  <si>
-    <t>64FB1-A7C8A-D74-DB8</t>
-  </si>
-  <si>
-    <t>C01622135F5EF40E10646684687B8270</t>
-  </si>
-  <si>
-    <t>11082337</t>
-  </si>
-  <si>
-    <t>64FC5-41165-5D6-3BB</t>
-  </si>
-  <si>
-    <t>FED867E875EE7E62BADD93C4B17B4BBE</t>
-  </si>
-  <si>
-    <t>11096134</t>
-  </si>
-  <si>
-    <t>64FDB-F159E-79E-038</t>
-  </si>
-  <si>
-    <t>6B048F9AE4BAA59788A02EFFF74310D3</t>
-  </si>
-  <si>
-    <t>Operadora - Operadora: VR - Sistema: Cielo&lt;br/&gt;Taxa - Operadora: 6,81 - Sistema: 2,32&lt;br/&gt;Valor Líquido - Operadora: 9,31 - Sistema: 0,00</t>
-  </si>
-  <si>
-    <t>11104464</t>
-  </si>
-  <si>
-    <t>64FF1-AB3A3-E4D-BF6</t>
-  </si>
-  <si>
-    <t>9BC101484C547842101FED2C34BA9204</t>
-  </si>
-  <si>
-    <t>Operadora - Operadora: Ticket - Sistema: Cielo&lt;br/&gt;Taxa - Operadora: 6,02 - Sistema: 2,32&lt;br/&gt;Valor Líquido - Operadora: 9,53 - Sistema: 0,00</t>
-  </si>
-  <si>
-    <t>11108858</t>
-  </si>
-  <si>
-    <t>65005-C7684-990-C99</t>
-  </si>
-  <si>
-    <t>351FE9D535C7DF757E4F5C0B30C92D11</t>
-  </si>
-  <si>
-    <t>11115004</t>
-  </si>
-  <si>
-    <t>65019-A327B-FEE-6EF</t>
-  </si>
-  <si>
-    <t>AF27F66082883F5765B5B36A3C21EA1D</t>
-  </si>
-  <si>
-    <t>11126261</t>
-  </si>
-  <si>
-    <t>65030-83F1B-D53-D15</t>
-  </si>
-  <si>
-    <t>6E01C8E62307266E17735C8B6F36C7DA</t>
-  </si>
-  <si>
-    <t>11138947</t>
-  </si>
-  <si>
-    <t>65045-4DEC1-12D-0A3</t>
-  </si>
-  <si>
-    <t>C20519E1E9FDEAB8181D243CE09685C1</t>
-  </si>
-  <si>
-    <t>11147494</t>
-  </si>
-  <si>
-    <t>65059-B42BA-D19-FD1</t>
-  </si>
-  <si>
-    <t>BC65C502E5110C98366953A867BD5EA</t>
-  </si>
-  <si>
-    <t>11154373</t>
-  </si>
-  <si>
-    <t>6506E-6FEE7-A0D-AA9</t>
-  </si>
-  <si>
-    <t>51B7EA171FDCF7F2B064FBFBC57AF911</t>
-  </si>
-  <si>
-    <t>11162057</t>
-  </si>
-  <si>
-    <t>65083-5B30F-D08-3F1</t>
-  </si>
-  <si>
-    <t>Pacote de 100.00 créditos</t>
-  </si>
-  <si>
-    <t>2947085C7B7D47C8A6C52C593B7A1B</t>
-  </si>
-  <si>
-    <t>11165975</t>
-  </si>
-  <si>
-    <t>6508A-EE673-40D-D9F</t>
-  </si>
-  <si>
-    <t>7B5F9F537E4A95B3CD73C46CCEEBE5D6</t>
-  </si>
-  <si>
-    <t>11170321</t>
-  </si>
-  <si>
-    <t>65098-957DA-3C7-FE6</t>
-  </si>
-  <si>
-    <t>735E439D4ADEBD265FCC7C71E8E54F25</t>
-  </si>
-  <si>
-    <t>11185239</t>
-  </si>
-  <si>
-    <t>650AF-98F68-B49-7F0</t>
-  </si>
-  <si>
-    <t>ED0EE50944F264F593925EB221C5D9E7</t>
-  </si>
-  <si>
-    <t>11192642</t>
-  </si>
-  <si>
-    <t>650C4-464BC-F67-D2F</t>
-  </si>
-  <si>
-    <t>FE3753775779E0EBE4F528393773DF2F</t>
-  </si>
-  <si>
-    <t>11199885</t>
-  </si>
-  <si>
-    <t>650D8-B0D5C-340-CF1</t>
-  </si>
-  <si>
-    <t>MAESTRO</t>
-  </si>
-  <si>
-    <t>3216354</t>
-  </si>
-  <si>
-    <t>2132132132</t>
-  </si>
-  <si>
-    <t>2754394</t>
-  </si>
-  <si>
-    <t>ELO CREDITO</t>
-  </si>
-  <si>
-    <t>32165416</t>
-  </si>
-  <si>
-    <t>32154651</t>
-  </si>
-  <si>
-    <t>2754397</t>
-  </si>
-  <si>
-    <t>32165132</t>
-  </si>
-  <si>
-    <t>3213431</t>
-  </si>
-  <si>
-    <t>2754400</t>
-  </si>
-  <si>
-    <t>1314351</t>
-  </si>
-  <si>
-    <t>3215431</t>
-  </si>
-  <si>
-    <t>2754402</t>
-  </si>
-  <si>
-    <t>500052</t>
-  </si>
-  <si>
-    <t>1015620</t>
-  </si>
-  <si>
-    <t>01 / 08</t>
-  </si>
-  <si>
-    <t>PDV</t>
-  </si>
-  <si>
-    <t>20002304242023002</t>
-  </si>
-  <si>
-    <t>500055</t>
-  </si>
-  <si>
-    <t>1015622</t>
-  </si>
-  <si>
-    <t>20002304342023002</t>
-  </si>
-  <si>
-    <t>500059</t>
-  </si>
-  <si>
-    <t>2010906</t>
-  </si>
-  <si>
-    <t>01 / 03</t>
-  </si>
-  <si>
-    <t>20002304582023002</t>
-  </si>
-  <si>
-    <t>20002304242023004</t>
-  </si>
-  <si>
-    <t>02 / 08</t>
-  </si>
-  <si>
-    <t>20002304242023005</t>
-  </si>
-  <si>
-    <t>03 / 08</t>
-  </si>
-  <si>
-    <t>20002304242023006</t>
-  </si>
-  <si>
-    <t>04 / 08</t>
-  </si>
-  <si>
-    <t>20002304242023007</t>
-  </si>
-  <si>
-    <t>05 / 08</t>
-  </si>
-  <si>
-    <t>20002304242023008</t>
-  </si>
-  <si>
-    <t>06 / 08</t>
-  </si>
-  <si>
-    <t>20002304242023009</t>
-  </si>
-  <si>
-    <t>07 / 08</t>
-  </si>
-  <si>
-    <t>20002304242023010</t>
-  </si>
-  <si>
-    <t>20002304582023004</t>
-  </si>
-  <si>
-    <t>02 / 03</t>
-  </si>
-  <si>
-    <t>20002304582023005</t>
-  </si>
-  <si>
-    <t>500098</t>
-  </si>
-  <si>
-    <t>2010932</t>
-  </si>
-  <si>
-    <t>01 / 04</t>
-  </si>
-  <si>
-    <t>20002306782023003</t>
-  </si>
-  <si>
-    <t>02 / 04</t>
-  </si>
-  <si>
-    <t>20002306782023004</t>
-  </si>
-  <si>
-    <t>03 / 04</t>
-  </si>
-  <si>
-    <t>20002306782023005</t>
-  </si>
-  <si>
-    <t>04 / 04</t>
-  </si>
-  <si>
-    <t>20002306782023006</t>
-  </si>
-  <si>
-    <t>MASTER CREDITO</t>
-  </si>
-  <si>
-    <t>AMEX - STONE</t>
-  </si>
-  <si>
-    <t>0000000001</t>
-  </si>
-  <si>
-    <t>9634</t>
-  </si>
-  <si>
-    <t>0000000123</t>
-  </si>
-  <si>
-    <t>9632</t>
-  </si>
-  <si>
-    <t>VISA ELECTRON DEBITO A VISTA</t>
-  </si>
-  <si>
-    <t>MASTERCARD CRED - GETNET</t>
-  </si>
-  <si>
-    <t>0000189852</t>
-  </si>
-  <si>
-    <t>9683</t>
-  </si>
-  <si>
-    <t>0000432268</t>
-  </si>
-  <si>
-    <t>9684</t>
-  </si>
-  <si>
-    <t>MASTERCARD DEB - GETNET</t>
-  </si>
-  <si>
-    <t>0000fr6rY6</t>
-  </si>
-  <si>
-    <t>9685</t>
-  </si>
-  <si>
-    <t>ELO DEBITO - GETNET</t>
-  </si>
-  <si>
-    <t>0000001234</t>
-  </si>
-  <si>
-    <t>9633</t>
-  </si>
-  <si>
-    <t>0000000002</t>
-  </si>
-  <si>
-    <t>9635</t>
-  </si>
-  <si>
-    <t>VISA CREDITO - GETNET</t>
-  </si>
-  <si>
-    <t>0000864432</t>
-  </si>
-  <si>
-    <t>9686</t>
-  </si>
-  <si>
-    <t>86D53E69155262C8FCFD2EF63FE27853</t>
-  </si>
-  <si>
-    <t>11220347</t>
-  </si>
-  <si>
-    <t>65117-34715-511-D1B</t>
-  </si>
-  <si>
-    <t>8C117FEA9E2E4B6EA2A5BB2262966F03</t>
-  </si>
-  <si>
-    <t>11230786</t>
-  </si>
-  <si>
-    <t>6512C-F1AB6-4FF-89A</t>
-  </si>
-  <si>
-    <t>71126DC5F86386E887EA54EB75D55444</t>
-  </si>
-  <si>
-    <t>11237663</t>
-  </si>
-  <si>
-    <t>65140-BA551-908-7FE</t>
-  </si>
-  <si>
-    <t>Pacote de 30.00 créditos</t>
-  </si>
-  <si>
-    <t>E4011FFE1B19AE5675F9D9FFF9A82CB3</t>
-  </si>
-  <si>
-    <t>11242936</t>
-  </si>
-  <si>
-    <t>65147-EDB3D-EBB-FA1</t>
-  </si>
-  <si>
-    <t>7BD2C04EC6750CF97ABAFD08743345E7</t>
-  </si>
-  <si>
-    <t>11248727</t>
-  </si>
-  <si>
-    <t>65156-51066-6A4-634</t>
-  </si>
-  <si>
-    <t>DB0C5D02EC4F40182EF0C1678436CD1D</t>
-  </si>
-  <si>
-    <t>11255547</t>
-  </si>
-  <si>
-    <t>6516B-D62C1-03E-3BA</t>
-  </si>
-  <si>
-    <t>32D1FF57C3465172B62CC82F402F0622</t>
-  </si>
-  <si>
-    <t>11268176</t>
-  </si>
-  <si>
-    <t>65181-BFD43-DD8-D65</t>
   </si>
   <si>
     <t>4.368,04</t>
@@ -708,7 +708,7 @@
     <col width="11.29" min="3" max="3" customWidth="1"/>
     <col width="18" min="4" max="4" customWidth="1"/>
     <col width="13.86" min="5" max="5" customWidth="1"/>
-    <col width="20.14" min="6" max="6" customWidth="1"/>
+    <col width="22.14" min="6" max="6" customWidth="1"/>
     <col width="15.86" min="7" max="7" customWidth="1"/>
     <col width="33.14" min="8" max="8" customWidth="1"/>
     <col width="11.57" min="9" max="9" customWidth="1"/>
@@ -716,7 +716,7 @@
     <col width="13" min="11" max="11" customWidth="1"/>
     <col width="12.14" min="12" max="12" customWidth="1"/>
     <col width="13.29" min="13" max="13" customWidth="1"/>
-    <col width="38" min="14" max="14" customWidth="1"/>
+    <col width="35.57" min="14" max="14" customWidth="1"/>
     <col width="12.71" min="15" max="15" customWidth="1"/>
     <col width="17" min="16" max="16" customWidth="1"/>
     <col width="9.29" min="17" max="17" customWidth="1"/>
@@ -799,10 +799,10 @@
         <v>22</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>45175</v>
+        <v>45199</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>45206</v>
+        <v>45230</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>23</v>
@@ -845,9 +845,7 @@
       <c r="S2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="5" t="n">
-        <v>8.67</v>
-      </c>
+      <c r="T2" s="5" t="n"/>
       <c r="U2" s="3" t="s"/>
     </row>
     <row r="3" spans="1:21" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -886,21 +884,21 @@
         <v>37</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q3" s="3" t="s"/>
       <c r="R3" s="3" t="s"/>
       <c r="S3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="T3" s="5" t="n"/>
       <c r="U3" s="3" t="s"/>
@@ -919,13 +917,13 @@
         <v>45207</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="H4" s="3" t="s"/>
       <c r="I4" s="5" t="n">
@@ -941,21 +939,21 @@
         <v>37</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q4" s="3" t="s"/>
       <c r="R4" s="3" t="s"/>
       <c r="S4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T4" s="5" t="n"/>
       <c r="U4" s="3" t="s"/>
@@ -983,7 +981,7 @@
         <v>25</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>9.9</v>
@@ -998,21 +996,21 @@
         <v>27</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O5" s="3" t="s"/>
       <c r="P5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R5" s="3" t="s"/>
       <c r="S5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T5" s="5" t="n"/>
       <c r="U5" s="3" t="s"/>
@@ -1040,7 +1038,7 @@
         <v>25</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>9.9</v>
@@ -1055,21 +1053,21 @@
         <v>27</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O6" s="3" t="s"/>
       <c r="P6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R6" s="3" t="s"/>
       <c r="S6" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="T6" s="5" t="n"/>
       <c r="U6" s="3" t="s"/>
@@ -1097,7 +1095,7 @@
         <v>25</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" s="5" t="n">
         <v>9.9</v>
@@ -1112,21 +1110,21 @@
         <v>27</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O7" s="3" t="s"/>
       <c r="P7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R7" s="3" t="s"/>
       <c r="S7" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T7" s="5" t="n"/>
       <c r="U7" s="3" t="s"/>
@@ -1139,25 +1137,25 @@
         <v>22</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>45180</v>
+        <v>45196</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>45211</v>
+        <v>45227</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>9.9</v>
+        <v>30</v>
       </c>
       <c r="J8" s="6" t="n">
         <v>2.32</v>
@@ -1172,22 +1170,20 @@
         <v>28</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="O8" s="3" t="s"/>
       <c r="P8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R8" s="3" t="s"/>
       <c r="S8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="T8" s="5" t="n">
-        <v>9.31</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="T8" s="5" t="n"/>
       <c r="U8" s="3" t="s"/>
     </row>
     <row r="9" spans="1:21" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -1198,10 +1194,10 @@
         <v>22</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>45181</v>
+        <v>45197</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>45212</v>
+        <v>45228</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>23</v>
@@ -1213,7 +1209,7 @@
         <v>25</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>9.9</v>
@@ -1231,22 +1227,20 @@
         <v>28</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="O9" s="3" t="s"/>
       <c r="P9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="R9" s="3" t="s"/>
       <c r="S9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="T9" s="5" t="n">
-        <v>9.53</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="T9" s="5" t="n"/>
       <c r="U9" s="3" t="s"/>
     </row>
     <row r="10" spans="1:21" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -1257,10 +1251,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>45182</v>
+        <v>45198</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>45213</v>
+        <v>45229</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>23</v>
@@ -1272,7 +1266,7 @@
         <v>25</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I10" s="5" t="n">
         <v>9.9</v>
@@ -1287,21 +1281,21 @@
         <v>27</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O10" s="3" t="s"/>
       <c r="P10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R10" s="3" t="s"/>
       <c r="S10" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T10" s="5" t="n"/>
       <c r="U10" s="3" t="s"/>
@@ -1314,10 +1308,10 @@
         <v>22</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>45183</v>
+        <v>45182</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>45214</v>
+        <v>45213</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>23</v>
@@ -1329,7 +1323,7 @@
         <v>25</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I11" s="5" t="n">
         <v>9.9</v>
@@ -1344,21 +1338,21 @@
         <v>27</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O11" s="3" t="s"/>
       <c r="P11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R11" s="3" t="s"/>
       <c r="S11" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="T11" s="5" t="n"/>
       <c r="U11" s="3" t="s"/>
@@ -1371,10 +1365,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>45184</v>
+        <v>45183</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>45215</v>
+        <v>45214</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>23</v>
@@ -1386,7 +1380,7 @@
         <v>25</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I12" s="5" t="n">
         <v>9.9</v>
@@ -1401,21 +1395,21 @@
         <v>27</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O12" s="3" t="s"/>
       <c r="P12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="R12" s="3" t="s"/>
       <c r="S12" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="T12" s="5" t="n"/>
       <c r="U12" s="3" t="s"/>
@@ -1428,10 +1422,10 @@
         <v>22</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>45185</v>
+        <v>45184</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>45216</v>
+        <v>45215</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>23</v>
@@ -1443,7 +1437,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I13" s="5" t="n">
         <v>9.9</v>
@@ -1458,21 +1452,21 @@
         <v>27</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O13" s="3" t="s"/>
       <c r="P13" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R13" s="3" t="s"/>
       <c r="S13" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="T13" s="5" t="n"/>
       <c r="U13" s="3" t="s"/>
@@ -1485,10 +1479,10 @@
         <v>22</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>45186</v>
+        <v>45185</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>45217</v>
+        <v>45216</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>23</v>
@@ -1500,7 +1494,7 @@
         <v>25</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I14" s="5" t="n">
         <v>9.9</v>
@@ -1515,21 +1509,21 @@
         <v>27</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O14" s="3" t="s"/>
       <c r="P14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="R14" s="3" t="s"/>
       <c r="S14" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="T14" s="5" t="n"/>
       <c r="U14" s="3" t="s"/>
@@ -1542,10 +1536,10 @@
         <v>22</v>
       </c>
       <c r="C15" s="4" t="n">
-        <v>45187</v>
+        <v>45186</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>45218</v>
+        <v>45217</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>23</v>
@@ -1557,7 +1551,7 @@
         <v>25</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I15" s="5" t="n">
         <v>9.9</v>
@@ -1572,21 +1566,21 @@
         <v>27</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O15" s="3" t="s"/>
       <c r="P15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="R15" s="3" t="s"/>
       <c r="S15" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="T15" s="5" t="n"/>
       <c r="U15" s="3" t="s"/>
@@ -1608,16 +1602,16 @@
         <v>23</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>100</v>
+        <v>9.9</v>
       </c>
       <c r="J16" s="6" t="n">
         <v>2.32</v>
@@ -1629,21 +1623,21 @@
         <v>27</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O16" s="3" t="s"/>
       <c r="P16" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="R16" s="3" t="s"/>
       <c r="S16" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="T16" s="5" t="n"/>
       <c r="U16" s="3" t="s"/>
@@ -1656,25 +1650,25 @@
         <v>22</v>
       </c>
       <c r="C17" s="4" t="n">
-        <v>45188</v>
+        <v>45187</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>45219</v>
+        <v>45218</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>9.9</v>
+        <v>100</v>
       </c>
       <c r="J17" s="6" t="n">
         <v>2.32</v>
@@ -1686,21 +1680,21 @@
         <v>27</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O17" s="3" t="s"/>
       <c r="P17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="R17" s="3" t="s"/>
       <c r="S17" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T17" s="5" t="n"/>
       <c r="U17" s="3" t="s"/>
@@ -1713,10 +1707,10 @@
         <v>22</v>
       </c>
       <c r="C18" s="4" t="n">
-        <v>45189</v>
+        <v>45188</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>45220</v>
+        <v>45219</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>23</v>
@@ -1728,7 +1722,7 @@
         <v>25</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I18" s="5" t="n">
         <v>9.9</v>
@@ -1743,21 +1737,21 @@
         <v>27</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O18" s="3" t="s"/>
       <c r="P18" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R18" s="3" t="s"/>
       <c r="S18" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="T18" s="5" t="n"/>
       <c r="U18" s="3" t="s"/>
@@ -1770,10 +1764,10 @@
         <v>22</v>
       </c>
       <c r="C19" s="4" t="n">
-        <v>45190</v>
+        <v>45189</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>45221</v>
+        <v>45220</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>23</v>
@@ -1785,7 +1779,7 @@
         <v>25</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I19" s="5" t="n">
         <v>9.9</v>
@@ -1800,21 +1794,21 @@
         <v>27</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O19" s="3" t="s"/>
       <c r="P19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="R19" s="3" t="s"/>
       <c r="S19" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T19" s="5" t="n"/>
       <c r="U19" s="3" t="s"/>
@@ -1827,10 +1821,10 @@
         <v>22</v>
       </c>
       <c r="C20" s="4" t="n">
-        <v>45191</v>
+        <v>45190</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>45222</v>
+        <v>45221</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>23</v>
@@ -1842,7 +1836,7 @@
         <v>25</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I20" s="5" t="n">
         <v>9.9</v>
@@ -1857,21 +1851,21 @@
         <v>27</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O20" s="3" t="s"/>
       <c r="P20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="R20" s="3" t="s"/>
       <c r="S20" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="T20" s="5" t="n"/>
       <c r="U20" s="3" t="s"/>
@@ -1880,7 +1874,9 @@
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="3" t="s"/>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C21" s="4" t="n">
         <v>45191</v>
       </c>
@@ -1888,41 +1884,45 @@
         <v>45222</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="3" t="s"/>
+        <v>23</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="G21" s="3" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>110.26</v>
+        <v>9.9</v>
       </c>
       <c r="J21" s="6" t="n">
-        <v>4</v>
+        <v>2.32</v>
       </c>
       <c r="K21" s="5" t="n">
-        <v>105.85</v>
+        <v>0</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O21" s="3" t="s"/>
       <c r="P21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q21" s="3" t="s"/>
+        <v>30</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="R21" s="3" t="s"/>
       <c r="S21" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="T21" s="5" t="n"/>
       <c r="U21" s="3" t="s"/>
@@ -1939,41 +1939,41 @@
         <v>45222</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F22" s="3" t="s"/>
       <c r="G22" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I22" s="5" t="n">
         <v>110.26</v>
       </c>
       <c r="J22" s="6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>104.75</v>
+        <v>105.85</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>37</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O22" s="3" t="s"/>
       <c r="P22" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q22" s="3" t="s"/>
       <c r="R22" s="3" t="s"/>
       <c r="S22" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="T22" s="5" t="n"/>
       <c r="U22" s="3" t="s"/>
@@ -1994,37 +1994,37 @@
       </c>
       <c r="F23" s="3" t="s"/>
       <c r="G23" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>100</v>
+        <v>110.26</v>
       </c>
       <c r="J23" s="6" t="n">
         <v>5</v>
       </c>
       <c r="K23" s="5" t="n">
-        <v>95</v>
+        <v>104.75</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>37</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O23" s="3" t="s"/>
       <c r="P23" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q23" s="3" t="s"/>
       <c r="R23" s="3" t="s"/>
       <c r="S23" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="T23" s="5" t="n"/>
       <c r="U23" s="3" t="s"/>
@@ -2045,10 +2045,10 @@
       </c>
       <c r="F24" s="3" t="s"/>
       <c r="G24" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I24" s="5" t="n">
         <v>100</v>
@@ -2063,19 +2063,19 @@
         <v>37</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O24" s="3" t="s"/>
       <c r="P24" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q24" s="3" t="s"/>
       <c r="R24" s="3" t="s"/>
       <c r="S24" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="T24" s="5" t="n"/>
       <c r="U24" s="3" t="s"/>
@@ -2086,47 +2086,47 @@
       </c>
       <c r="B25" s="3" t="s"/>
       <c r="C25" s="4" t="n">
-        <v>45192</v>
+        <v>45191</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>45252</v>
+        <v>45222</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="F25" s="3" t="s"/>
       <c r="G25" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I25" s="5" t="n">
-        <v>181.52</v>
+        <v>100</v>
       </c>
       <c r="J25" s="6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K25" s="5" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O25" s="3" t="s"/>
       <c r="P25" s="3" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="Q25" s="3" t="s"/>
       <c r="R25" s="3" t="s"/>
       <c r="S25" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="T25" s="5" t="n"/>
       <c r="U25" s="3" t="s"/>
@@ -2147,13 +2147,13 @@
       </c>
       <c r="F26" s="3" t="s"/>
       <c r="G26" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>181.39</v>
+        <v>181.52</v>
       </c>
       <c r="J26" s="6" t="n">
         <v>0</v>
@@ -2162,13 +2162,13 @@
         <v>0</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O26" s="3" t="s"/>
       <c r="P26" s="3" t="s">
@@ -2177,7 +2177,7 @@
       <c r="Q26" s="3" t="s"/>
       <c r="R26" s="3" t="s"/>
       <c r="S26" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="T26" s="5" t="n"/>
       <c r="U26" s="3" t="s"/>
@@ -2198,13 +2198,13 @@
       </c>
       <c r="F27" s="3" t="s"/>
       <c r="G27" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I27" s="5" t="n">
-        <v>124.88</v>
+        <v>181.39</v>
       </c>
       <c r="J27" s="6" t="n">
         <v>0</v>
@@ -2213,13 +2213,13 @@
         <v>0</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O27" s="3" t="s"/>
       <c r="P27" s="3" t="s">
@@ -2228,7 +2228,7 @@
       <c r="Q27" s="3" t="s"/>
       <c r="R27" s="3" t="s"/>
       <c r="S27" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="T27" s="5" t="n"/>
       <c r="U27" s="3" t="s"/>
@@ -2242,20 +2242,20 @@
         <v>45192</v>
       </c>
       <c r="D28" s="4" t="n">
-        <v>45312</v>
+        <v>45252</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F28" s="3" t="s"/>
       <c r="G28" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="I28" s="5" t="n">
-        <v>181.52</v>
+        <v>124.88</v>
       </c>
       <c r="J28" s="6" t="n">
         <v>0</v>
@@ -2264,13 +2264,13 @@
         <v>0</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O28" s="3" t="s"/>
       <c r="P28" s="3" t="s">
@@ -2279,7 +2279,7 @@
       <c r="Q28" s="3" t="s"/>
       <c r="R28" s="3" t="s"/>
       <c r="S28" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T28" s="5" t="n"/>
       <c r="U28" s="3" t="s"/>
@@ -2293,7 +2293,7 @@
         <v>45192</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>45342</v>
+        <v>45312</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>23</v>
@@ -2315,13 +2315,13 @@
         <v>0</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O29" s="3" t="s"/>
       <c r="P29" s="3" t="s">
@@ -2330,7 +2330,7 @@
       <c r="Q29" s="3" t="s"/>
       <c r="R29" s="3" t="s"/>
       <c r="S29" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="T29" s="5" t="n"/>
       <c r="U29" s="3" t="s"/>
@@ -2344,7 +2344,7 @@
         <v>45192</v>
       </c>
       <c r="D30" s="4" t="n">
-        <v>45372</v>
+        <v>45342</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>23</v>
@@ -2366,13 +2366,13 @@
         <v>0</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O30" s="3" t="s"/>
       <c r="P30" s="3" t="s">
@@ -2381,7 +2381,7 @@
       <c r="Q30" s="3" t="s"/>
       <c r="R30" s="3" t="s"/>
       <c r="S30" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T30" s="5" t="n"/>
       <c r="U30" s="3" t="s"/>
@@ -2395,7 +2395,7 @@
         <v>45192</v>
       </c>
       <c r="D31" s="4" t="n">
-        <v>45402</v>
+        <v>45372</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>23</v>
@@ -2417,13 +2417,13 @@
         <v>0</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O31" s="3" t="s"/>
       <c r="P31" s="3" t="s">
@@ -2432,7 +2432,7 @@
       <c r="Q31" s="3" t="s"/>
       <c r="R31" s="3" t="s"/>
       <c r="S31" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="T31" s="5" t="n"/>
       <c r="U31" s="3" t="s"/>
@@ -2446,7 +2446,7 @@
         <v>45192</v>
       </c>
       <c r="D32" s="4" t="n">
-        <v>45432</v>
+        <v>45402</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>23</v>
@@ -2468,13 +2468,13 @@
         <v>0</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O32" s="3" t="s"/>
       <c r="P32" s="3" t="s">
@@ -2483,7 +2483,7 @@
       <c r="Q32" s="3" t="s"/>
       <c r="R32" s="3" t="s"/>
       <c r="S32" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="T32" s="5" t="n"/>
       <c r="U32" s="3" t="s"/>
@@ -2497,7 +2497,7 @@
         <v>45192</v>
       </c>
       <c r="D33" s="4" t="n">
-        <v>45462</v>
+        <v>45432</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>23</v>
@@ -2519,13 +2519,13 @@
         <v>0</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O33" s="3" t="s"/>
       <c r="P33" s="3" t="s">
@@ -2534,7 +2534,7 @@
       <c r="Q33" s="3" t="s"/>
       <c r="R33" s="3" t="s"/>
       <c r="S33" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="T33" s="5" t="n"/>
       <c r="U33" s="3" t="s"/>
@@ -2548,7 +2548,7 @@
         <v>45192</v>
       </c>
       <c r="D34" s="4" t="n">
-        <v>45492</v>
+        <v>45462</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>23</v>
@@ -2561,7 +2561,7 @@
         <v>113</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>181.55</v>
+        <v>181.52</v>
       </c>
       <c r="J34" s="6" t="n">
         <v>0</v>
@@ -2570,13 +2570,13 @@
         <v>0</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O34" s="3" t="s"/>
       <c r="P34" s="3" t="s">
@@ -2585,7 +2585,7 @@
       <c r="Q34" s="3" t="s"/>
       <c r="R34" s="3" t="s"/>
       <c r="S34" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="T34" s="5" t="n"/>
       <c r="U34" s="3" t="s"/>
@@ -2599,20 +2599,20 @@
         <v>45192</v>
       </c>
       <c r="D35" s="4" t="n">
-        <v>45312</v>
+        <v>45492</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F35" s="3" t="s"/>
       <c r="G35" s="3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I35" s="5" t="n">
-        <v>124.88</v>
+        <v>181.55</v>
       </c>
       <c r="J35" s="6" t="n">
         <v>0</v>
@@ -2621,13 +2621,13 @@
         <v>0</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O35" s="3" t="s"/>
       <c r="P35" s="3" t="s">
@@ -2636,7 +2636,7 @@
       <c r="Q35" s="3" t="s"/>
       <c r="R35" s="3" t="s"/>
       <c r="S35" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T35" s="5" t="n"/>
       <c r="U35" s="3" t="s"/>
@@ -2650,7 +2650,7 @@
         <v>45192</v>
       </c>
       <c r="D36" s="4" t="n">
-        <v>45342</v>
+        <v>45312</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>23</v>
@@ -2672,13 +2672,13 @@
         <v>0</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O36" s="3" t="s"/>
       <c r="P36" s="3" t="s">
@@ -2687,7 +2687,7 @@
       <c r="Q36" s="3" t="s"/>
       <c r="R36" s="3" t="s"/>
       <c r="S36" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="T36" s="5" t="n"/>
       <c r="U36" s="3" t="s"/>
@@ -2701,20 +2701,20 @@
         <v>45192</v>
       </c>
       <c r="D37" s="4" t="n">
-        <v>45282</v>
+        <v>45342</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F37" s="3" t="s"/>
       <c r="G37" s="3" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="I37" s="5" t="n">
-        <v>142.54</v>
+        <v>124.88</v>
       </c>
       <c r="J37" s="6" t="n">
         <v>0</v>
@@ -2723,13 +2723,13 @@
         <v>0</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O37" s="3" t="s"/>
       <c r="P37" s="3" t="s">
@@ -2738,7 +2738,7 @@
       <c r="Q37" s="3" t="s"/>
       <c r="R37" s="3" t="s"/>
       <c r="S37" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="T37" s="5" t="n"/>
       <c r="U37" s="3" t="s"/>
@@ -2752,7 +2752,7 @@
         <v>45192</v>
       </c>
       <c r="D38" s="4" t="n">
-        <v>45312</v>
+        <v>45282</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>23</v>
@@ -2774,13 +2774,13 @@
         <v>0</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O38" s="3" t="s"/>
       <c r="P38" s="3" t="s">
@@ -2789,7 +2789,7 @@
       <c r="Q38" s="3" t="s"/>
       <c r="R38" s="3" t="s"/>
       <c r="S38" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="T38" s="5" t="n"/>
       <c r="U38" s="3" t="s"/>
@@ -2803,7 +2803,7 @@
         <v>45192</v>
       </c>
       <c r="D39" s="4" t="n">
-        <v>45342</v>
+        <v>45312</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>23</v>
@@ -2825,13 +2825,13 @@
         <v>0</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O39" s="3" t="s"/>
       <c r="P39" s="3" t="s">
@@ -2840,7 +2840,7 @@
       <c r="Q39" s="3" t="s"/>
       <c r="R39" s="3" t="s"/>
       <c r="S39" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="T39" s="5" t="n"/>
       <c r="U39" s="3" t="s"/>
@@ -2854,7 +2854,7 @@
         <v>45192</v>
       </c>
       <c r="D40" s="4" t="n">
-        <v>45372</v>
+        <v>45342</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>23</v>
@@ -2867,7 +2867,7 @@
         <v>141</v>
       </c>
       <c r="I40" s="5" t="n">
-        <v>142.55</v>
+        <v>142.54</v>
       </c>
       <c r="J40" s="6" t="n">
         <v>0</v>
@@ -2876,13 +2876,13 @@
         <v>0</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O40" s="3" t="s"/>
       <c r="P40" s="3" t="s">
@@ -2891,7 +2891,7 @@
       <c r="Q40" s="3" t="s"/>
       <c r="R40" s="3" t="s"/>
       <c r="S40" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="T40" s="5" t="n"/>
       <c r="U40" s="3" t="s"/>
@@ -2900,27 +2900,25 @@
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="B41" s="3" t="s"/>
       <c r="C41" s="4" t="n">
-        <v>45194</v>
+        <v>45192</v>
       </c>
       <c r="D41" s="4" t="n">
-        <v>45224</v>
+        <v>45372</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>151</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F41" s="3" t="s"/>
       <c r="G41" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="H41" s="3" t="s"/>
+        <v>140</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="I41" s="5" t="n">
-        <v>8.5</v>
+        <v>142.55</v>
       </c>
       <c r="J41" s="6" t="n">
         <v>0</v>
@@ -2929,24 +2927,22 @@
         <v>0</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>37</v>
+        <v>148</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O41" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="O41" s="3" t="s"/>
       <c r="P41" s="3" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="Q41" s="3" t="s"/>
       <c r="R41" s="3" t="s"/>
       <c r="S41" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="T41" s="5" t="n"/>
       <c r="U41" s="3" t="s"/>
@@ -2965,20 +2961,20 @@
         <v>45224</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>43</v>
+        <v>150</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H42" s="3" t="s"/>
       <c r="I42" s="5" t="n">
-        <v>19.9</v>
+        <v>8.5</v>
       </c>
       <c r="J42" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K42" s="5" t="n">
         <v>0</v>
@@ -2987,21 +2983,21 @@
         <v>37</v>
       </c>
       <c r="M42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O42" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N42" s="3" t="s">
+      <c r="P42" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="O42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P42" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q42" s="3" t="s"/>
       <c r="R42" s="3" t="s"/>
       <c r="S42" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="T42" s="5" t="n"/>
       <c r="U42" s="3" t="s"/>
@@ -3020,20 +3016,20 @@
         <v>45224</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>156</v>
+        <v>41</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>157</v>
+        <v>42</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H43" s="3" t="s"/>
       <c r="I43" s="5" t="n">
-        <v>30</v>
+        <v>19.9</v>
       </c>
       <c r="J43" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K43" s="5" t="n">
         <v>0</v>
@@ -3042,21 +3038,21 @@
         <v>37</v>
       </c>
       <c r="M43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O43" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N43" s="3" t="s">
+      <c r="P43" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="O43" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P43" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q43" s="3" t="s"/>
       <c r="R43" s="3" t="s"/>
       <c r="S43" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="T43" s="5" t="n"/>
       <c r="U43" s="3" t="s"/>
@@ -3081,11 +3077,11 @@
         <v>157</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H44" s="3" t="s"/>
       <c r="I44" s="5" t="n">
-        <v>134.37</v>
+        <v>30</v>
       </c>
       <c r="J44" s="6" t="n">
         <v>0</v>
@@ -3097,21 +3093,21 @@
         <v>37</v>
       </c>
       <c r="M44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O44" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N44" s="3" t="s">
+      <c r="P44" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="O44" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P44" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q44" s="3" t="s"/>
       <c r="R44" s="3" t="s"/>
       <c r="S44" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T44" s="5" t="n"/>
       <c r="U44" s="3" t="s"/>
@@ -3127,23 +3123,23 @@
         <v>45194</v>
       </c>
       <c r="D45" s="4" t="n">
-        <v>45196</v>
+        <v>45224</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>156</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H45" s="3" t="s"/>
       <c r="I45" s="5" t="n">
-        <v>10</v>
+        <v>134.37</v>
       </c>
       <c r="J45" s="6" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="K45" s="5" t="n">
         <v>0</v>
@@ -3152,21 +3148,21 @@
         <v>37</v>
       </c>
       <c r="M45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O45" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N45" s="3" t="s">
+      <c r="P45" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="O45" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P45" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q45" s="3" t="s"/>
       <c r="R45" s="3" t="s"/>
       <c r="S45" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="T45" s="5" t="n"/>
       <c r="U45" s="3" t="s"/>
@@ -3185,20 +3181,20 @@
         <v>45196</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H46" s="3" t="s"/>
       <c r="I46" s="5" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="J46" s="6" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="K46" s="5" t="n">
         <v>0</v>
@@ -3207,21 +3203,21 @@
         <v>37</v>
       </c>
       <c r="M46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O46" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N46" s="3" t="s">
+      <c r="P46" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="O46" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P46" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q46" s="3" t="s"/>
       <c r="R46" s="3" t="s"/>
       <c r="S46" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="T46" s="5" t="n"/>
       <c r="U46" s="3" t="s"/>
@@ -3246,11 +3242,11 @@
         <v>165</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H47" s="3" t="s"/>
       <c r="I47" s="5" t="n">
-        <v>8.5</v>
+        <v>100</v>
       </c>
       <c r="J47" s="6" t="n">
         <v>0</v>
@@ -3262,21 +3258,21 @@
         <v>37</v>
       </c>
       <c r="M47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O47" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N47" s="3" t="s">
+      <c r="P47" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="O47" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P47" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q47" s="3" t="s"/>
       <c r="R47" s="3" t="s"/>
       <c r="S47" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T47" s="5" t="n"/>
       <c r="U47" s="3" t="s"/>
@@ -3295,20 +3291,20 @@
         <v>45196</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H48" s="3" t="s"/>
       <c r="I48" s="5" t="n">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="J48" s="6" t="n">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="K48" s="5" t="n">
         <v>0</v>
@@ -3317,21 +3313,21 @@
         <v>37</v>
       </c>
       <c r="M48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O48" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N48" s="3" t="s">
+      <c r="P48" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="O48" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P48" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q48" s="3" t="s"/>
       <c r="R48" s="3" t="s"/>
       <c r="S48" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="T48" s="5" t="n"/>
       <c r="U48" s="3" t="s"/>
@@ -3341,54 +3337,52 @@
         <v>21</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C49" s="4" t="n">
         <v>45194</v>
       </c>
       <c r="D49" s="4" t="n">
-        <v>45225</v>
+        <v>45196</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>24</v>
+        <v>170</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>173</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="H49" s="3" t="s"/>
       <c r="I49" s="5" t="n">
-        <v>9.9</v>
+        <v>10</v>
       </c>
       <c r="J49" s="6" t="n">
-        <v>2.32</v>
+        <v>1.4</v>
       </c>
       <c r="K49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="M49" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O49" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N49" s="3" t="s">
+      <c r="P49" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O49" s="3" t="s"/>
-      <c r="P49" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q49" s="3" t="s">
-        <v>174</v>
-      </c>
+      <c r="Q49" s="3" t="s"/>
       <c r="R49" s="3" t="s"/>
       <c r="S49" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="T49" s="5" t="n"/>
       <c r="U49" s="3" t="s"/>
@@ -3401,10 +3395,10 @@
         <v>22</v>
       </c>
       <c r="C50" s="4" t="n">
-        <v>45195</v>
+        <v>45194</v>
       </c>
       <c r="D50" s="4" t="n">
-        <v>45226</v>
+        <v>45225</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>23</v>
@@ -3416,7 +3410,7 @@
         <v>25</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I50" s="5" t="n">
         <v>9.9</v>
@@ -3431,21 +3425,21 @@
         <v>27</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O50" s="3" t="s"/>
       <c r="P50" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="R50" s="3" t="s"/>
       <c r="S50" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="T50" s="5" t="n"/>
       <c r="U50" s="3" t="s"/>
@@ -3458,10 +3452,10 @@
         <v>22</v>
       </c>
       <c r="C51" s="4" t="n">
-        <v>45196</v>
+        <v>45195</v>
       </c>
       <c r="D51" s="4" t="n">
-        <v>45227</v>
+        <v>45226</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>23</v>
@@ -3473,7 +3467,7 @@
         <v>25</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I51" s="5" t="n">
         <v>9.9</v>
@@ -3488,21 +3482,21 @@
         <v>27</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N51" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O51" s="3" t="s"/>
       <c r="P51" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="R51" s="3" t="s"/>
       <c r="S51" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="T51" s="5" t="n"/>
       <c r="U51" s="3" t="s"/>
@@ -3524,16 +3518,16 @@
         <v>23</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>182</v>
+        <v>24</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I52" s="5" t="n">
-        <v>30</v>
+        <v>9.9</v>
       </c>
       <c r="J52" s="6" t="n">
         <v>2.32</v>
@@ -3545,21 +3539,21 @@
         <v>27</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N52" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O52" s="3" t="s"/>
       <c r="P52" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R52" s="3" t="s"/>
       <c r="S52" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="T52" s="5" t="n"/>
       <c r="U52" s="3" t="s"/>
@@ -3572,10 +3566,10 @@
         <v>22</v>
       </c>
       <c r="C53" s="4" t="n">
-        <v>45197</v>
+        <v>45180</v>
       </c>
       <c r="D53" s="4" t="n">
-        <v>45228</v>
+        <v>45211</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>23</v>
@@ -3587,7 +3581,7 @@
         <v>25</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I53" s="5" t="n">
         <v>9.9</v>
@@ -3602,23 +3596,25 @@
         <v>27</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>39</v>
+        <v>184</v>
       </c>
       <c r="O53" s="3" t="s"/>
       <c r="P53" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="R53" s="3" t="s"/>
       <c r="S53" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="T53" s="5" t="n"/>
+        <v>186</v>
+      </c>
+      <c r="T53" s="5" t="n">
+        <v>9.31</v>
+      </c>
       <c r="U53" s="3" t="s"/>
     </row>
     <row r="54" spans="1:21" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -3629,10 +3625,10 @@
         <v>22</v>
       </c>
       <c r="C54" s="4" t="n">
-        <v>45198</v>
+        <v>45181</v>
       </c>
       <c r="D54" s="4" t="n">
-        <v>45229</v>
+        <v>45212</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>23</v>
@@ -3644,7 +3640,7 @@
         <v>25</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I54" s="5" t="n">
         <v>9.9</v>
@@ -3659,23 +3655,25 @@
         <v>27</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="O54" s="3" t="s"/>
       <c r="P54" s="3" t="s">
         <v>30</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R54" s="3" t="s"/>
       <c r="S54" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="T54" s="5" t="n"/>
+        <v>190</v>
+      </c>
+      <c r="T54" s="5" t="n">
+        <v>9.53</v>
+      </c>
       <c r="U54" s="3" t="s"/>
     </row>
     <row r="55" spans="1:21" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -3686,10 +3684,10 @@
         <v>22</v>
       </c>
       <c r="C55" s="4" t="n">
-        <v>45199</v>
+        <v>45175</v>
       </c>
       <c r="D55" s="4" t="n">
-        <v>45230</v>
+        <v>45206</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>23</v>
@@ -3701,7 +3699,7 @@
         <v>25</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I55" s="5" t="n">
         <v>9.9</v>
@@ -3716,10 +3714,10 @@
         <v>27</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>39</v>
+        <v>192</v>
       </c>
       <c r="O55" s="3" t="s"/>
       <c r="P55" s="3" t="s">
@@ -3732,7 +3730,9 @@
       <c r="S55" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="T55" s="5" t="n"/>
+      <c r="T55" s="5" t="n">
+        <v>8.67</v>
+      </c>
       <c r="U55" s="3" t="s"/>
     </row>
     <row r="56" spans="1:21" outlineLevel="0" x14ac:dyDescent="0.25">

</xml_diff>